<commit_message>
excel  coopro_proj have problem
</commit_message>
<xml_diff>
--- a/public/Excel_example/other/cooperation_proj.xlsx
+++ b/public/Excel_example/other/cooperation_proj.xlsx
@@ -14,47 +14,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>單位名稱</t>
-  </si>
-  <si>
-    <t>系所部門</t>
-  </si>
-  <si>
-    <t>主持人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>所屬一級</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>單位</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>所屬</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>系所部門</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>主辦人</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>合作機構</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>計畫名稱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>計畫內容</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>開始時間</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>結束時間</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>備註</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -66,6 +110,31 @@
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -90,8 +159,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -396,41 +471,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.25" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
other function upload  transnational_degree have problem
</commit_message>
<xml_diff>
--- a/public/Excel_example/other/cooperation_proj.xlsx
+++ b/public/Excel_example/other/cooperation_proj.xlsx
@@ -474,13 +474,13 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.25" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="14.375" customWidth="1"/>
+    <col min="2" max="2" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>